<commit_message>
Further assignment submission details
</commit_message>
<xml_diff>
--- a/Kaggle/IEEE/Datasets/Model Performance/PDB-CA2 Model Metrics cf v1-0 220423.xlsx
+++ b/Kaggle/IEEE/Datasets/Model Performance/PDB-CA2 Model Metrics cf v1-0 220423.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TU_D\Big Data\Assignment B\repo\Kaggle\IEEE\Datasets\Model Performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA9BEED-94A6-4297-AACC-91F67C904D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F56C753-53E0-4496-A69E-9CD8B4B5FE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{3F698C8D-2D52-4D99-A62D-9ABB8213BD8F}"/>
   </bookViews>
@@ -235,15 +235,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +255,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -271,6 +271,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -302,24 +320,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -340,13 +340,13 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10CD84DA-1F10-4CFA-8F7A-296762584ADC}" name="Table1" displayName="Table1" ref="B3:H7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="13">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E5432832-3CF8-4101-9A57-6521E1982527}" name="Column1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{B59943DE-2992-4166-A819-ADAD47DEC76D}" name="Models" headerRowDxfId="7" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{D76C40B8-5CD8-453B-B180-FE373245FFF3}" name="Column2" headerRowDxfId="8" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{F0285924-96A9-4FD3-AA6E-12FF3320CB67}" name="Column3" headerRowDxfId="9" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{3A31C285-4F95-4642-90A9-0E6EC0EF6B58}" name="Column4" headerRowDxfId="10" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{F2273CF2-37DB-495B-BF2E-D96FDD32DBA4}" name="Column5" headerRowDxfId="11" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{07B314BD-9231-4305-9654-2B46B72F0448}" name="Column6" headerRowDxfId="12" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E5432832-3CF8-4101-9A57-6521E1982527}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{B59943DE-2992-4166-A819-ADAD47DEC76D}" name="Models" headerRowDxfId="11" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{D76C40B8-5CD8-453B-B180-FE373245FFF3}" name="Column2" headerRowDxfId="9" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F0285924-96A9-4FD3-AA6E-12FF3320CB67}" name="Column3" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3A31C285-4F95-4642-90A9-0E6EC0EF6B58}" name="Column4" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F2273CF2-37DB-495B-BF2E-D96FDD32DBA4}" name="Column5" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{07B314BD-9231-4305-9654-2B46B72F0448}" name="Column6" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -652,7 +652,7 @@
   <dimension ref="B1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,41 +663,41 @@
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -705,92 +705,92 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <v>0.80810000000000004</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>0.78990000000000005</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="7">
         <v>0.76200000000000001</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <v>0.79369999999999996</v>
       </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
+      <c r="G4" s="7">
+        <v>0.74160000000000004</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.76219999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>0.76819999999999999</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>0.76290000000000002</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>0.72399999999999998</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <v>0.76429999999999998</v>
       </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0</v>
+      <c r="G5" s="9">
+        <v>0.69989999999999997</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.75829999999999997</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>0.88839999999999997</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>0.86250000000000004</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>0.84630000000000005</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <v>0.86890000000000001</v>
       </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
+      <c r="G6" s="9">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.84219999999999995</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <v>0.89959999999999996</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>0.87380000000000002</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.86040000000000005</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>0.8841</v>
       </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14">
-        <v>0</v>
+      <c r="G7" s="10">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.84909999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>